<commit_message>
more graphs for question 6
</commit_message>
<xml_diff>
--- a/Question6Data/Question6Data.xlsx
+++ b/Question6Data/Question6Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5132,6 +5132,2714 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Queue</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> Utilization (0.4, 10) vs. Average Packets in Buffer </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>K=10</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0.99192400000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.47373</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.09809</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9567999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9972699999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9942500000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.9601699999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.7157499999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.3289200000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.7793299999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.1275700000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.4177400000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.6011600000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.77881</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.9138599999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.0229900000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.1789100000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.2970699999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.3837600000000005</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.4526299999999992</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.5124899999999997</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.5540199999999995</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.5912600000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.6243700000000008</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.6518499999999996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.6761199999999992</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.6963699999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.7160600000000006</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9.7310099999999995</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9.7461099999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9.7601300000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.7819299999999991</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9.8010900000000003</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9.8181700000000003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.8319100000000006</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.8427900000000008</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9.8532799999999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9.8628400000000003</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9.8707100000000008</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9.8782899999999998</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9.8848500000000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9.8910599999999995</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9.8962199999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2420-47A8-930F-0E7A311A5935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>K=25</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>1.0064</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4840899999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3107799999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8355199999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.3347199999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.4131</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.4178</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.227799999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.700099999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.514099999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22.996400000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23.359100000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23.588200000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23.761399999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23.8977</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24.0045</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24.171900000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>24.2959</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24.384799999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>24.454000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>24.5108</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>24.556000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24.592300000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.623799999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.6526</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>24.676300000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>24.697600000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>24.7135</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>24.7316</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>24.746500000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>24.760300000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>24.782900000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>24.8017</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>24.8186</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>24.8309</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>24.8431</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>24.853400000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>24.863600000000002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>24.871099999999998</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>24.8781</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>24.885100000000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>24.8904</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>24.8962</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2420-47A8-930F-0E7A311A5935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>K=50</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$U$2:$U$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Y$2:$Y$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>1.00373</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.48855</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3279399999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.03538</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0661900000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.5654</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40.109699999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44.969499999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46.6539</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>47.460099999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>47.982300000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48.334800000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>48.576900000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>48.754600000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>48.898600000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>49.003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>49.173099999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>49.296900000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>49.389899999999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>49.453600000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>49.509300000000003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>49.553600000000003</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>49.594999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>49.622100000000003</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>49.652500000000003</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>49.677</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>49.697800000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>49.714799999999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>49.732999999999997</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>49.746099999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>49.759900000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>49.782499999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>49.801600000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>49.817399999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>49.831000000000003</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>49.8414</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>49.853299999999997</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>49.862499999999997</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>49.870399999999997</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>49.878</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>49.884300000000003</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>49.890300000000003</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>49.895600000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2420-47A8-930F-0E7A311A5935}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="843903199"/>
+        <c:axId val="843901951"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="843903199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="0.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Queue</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> Utilization</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="843901951"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="843901951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> Packets in Buffer</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="843903199"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Queue</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> Utilization (0.4, 10) vs. Packet Loss Probability </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>K=10</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>4.2735700000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.56807E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.1807800000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3024800000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0424900000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.0275400000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.14152000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.192828</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.245561</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.29206599999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.33617599999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.37725500000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.41334599999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.44644</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.47536699999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.50168699999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.54583499999999996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.58379899999999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.61512699999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.64287899999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.66690300000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.68756499999999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.70531299999999997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.72232499999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.73691399999999996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.749892</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.76160600000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.77285599999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.78260799999999997</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.79117000000000004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.80025299999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.81465100000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.82755500000000004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.839059</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.84923700000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.857074</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.86490599999999995</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.87217800000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.87820699999999996</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.88381399999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.88919400000000004</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.89413900000000002</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.89813699999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B0E-405C-94AA-EAD227A7203F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>K=25</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.6599200000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.6537599999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.7575200000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.95278E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.16683400000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.22964799999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.28650300000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.33300099999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.37346600000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.41205599999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.44424999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.47376699999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.499199</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.54517300000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.58303099999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.61591399999999996</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.64308200000000004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.666736</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.68811800000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.70561300000000005</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.72214800000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.73684499999999997</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.749502</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.76198600000000005</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.77253099999999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.78267399999999998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.79164900000000005</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.79985600000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.81492100000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.82811599999999996</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.83968200000000004</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.84848900000000005</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.85724999999999996</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.86489400000000005</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.87223099999999998</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.87836899999999996</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.88389399999999996</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.88915900000000003</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.89371599999999995</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.898393</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5B0E-405C-94AA-EAD227A7203F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>K=50</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$U$2:$U$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$W$2:$W$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>2.7466100000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.7475999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.89181E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.8152599999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.16652700000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.22827</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.28329900000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.33124500000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.37462699999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.41172799999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.444942</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.47371600000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.49914599999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.54522800000000005</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.58341299999999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.61624500000000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.64244400000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.66708699999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.68718100000000004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.70665999999999995</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.72167499999999996</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.73706199999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.750749</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.76196399999999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.77313500000000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.78365899999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.79170399999999996</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.80029899999999998</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.81528199999999995</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.82786800000000005</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.83935099999999996</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.84865500000000005</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.85675699999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.86511300000000002</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.87195</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.878135</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.88409700000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.88892300000000002</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.89370400000000005</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.89807499999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5B0E-405C-94AA-EAD227A7203F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="843903199"/>
+        <c:axId val="843901951"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="843903199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="0.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Queue</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> Utilization</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="843901951"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="843901951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Packet Loss Probability</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="843903199"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5372,6 +8080,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -7953,6 +10741,1038 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8655,6 +12475,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>111919</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>173037</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1262856</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>173037</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8928,8 +12812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="X65" sqref="X65"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="R101" sqref="R101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>